<commit_message>
Revert for Unity Changes and Update to Game Theory
</commit_message>
<xml_diff>
--- a/Game Theory.xlsx
+++ b/Game Theory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public-Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FE4A9C-AA34-4C12-ADD1-A46A55030804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070B660B-A915-4E60-A92E-7D5C51BB9D9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{A1BE79B9-B4EE-42B4-9FA0-1B70B1F5C2B2}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="12735" activeTab="6" xr2:uid="{A1BE79B9-B4EE-42B4-9FA0-1B70B1F5C2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Pure - Blend Class Chart" sheetId="1" r:id="rId4"/>
     <sheet name="Class Guides" sheetId="2" r:id="rId5"/>
     <sheet name="Equipment" sheetId="6" r:id="rId6"/>
-    <sheet name="Checklist" sheetId="7" r:id="rId7"/>
+    <sheet name="Advanced Combat" sheetId="8" r:id="rId7"/>
+    <sheet name="Checklist" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="441">
   <si>
     <t>Strength</t>
   </si>
@@ -1051,6 +1052,315 @@
   </si>
   <si>
     <t>UI and Menus</t>
+  </si>
+  <si>
+    <t>Royalty</t>
+  </si>
+  <si>
+    <t>Prince</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>Bishop</t>
+  </si>
+  <si>
+    <t>Shift Demon</t>
+  </si>
+  <si>
+    <t>Shift Dragon</t>
+  </si>
+  <si>
+    <t>Rotten</t>
+  </si>
+  <si>
+    <t>Elementals</t>
+  </si>
+  <si>
+    <t>Sun King</t>
+  </si>
+  <si>
+    <t>Dark Lord</t>
+  </si>
+  <si>
+    <t>Frost Knight</t>
+  </si>
+  <si>
+    <t>Flame Knight</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Lunar</t>
+  </si>
+  <si>
+    <t>Scryer</t>
+  </si>
+  <si>
+    <t>Elixir Master</t>
+  </si>
+  <si>
+    <t>Expanding Class to contain similar classes to others but using cheaper crafting materials</t>
+  </si>
+  <si>
+    <t>For example, the Elixir master could be a copy of a mage but with hard to craft materials but very low costs per spell</t>
+  </si>
+  <si>
+    <t>Scroll Master</t>
+  </si>
+  <si>
+    <t>Example, Scrollmaster is similar to a support but the crafting material is just paper. It would be slightly weaker, but good for farming</t>
+  </si>
+  <si>
+    <t>Some classes can be highly bound with few options but low costs. Same play style, same quests to earn the classes sometimes.</t>
+  </si>
+  <si>
+    <t>Just another way to differentiate classes without making everything about them different.</t>
+  </si>
+  <si>
+    <t>Storm King</t>
+  </si>
+  <si>
+    <t>Pirate</t>
+  </si>
+  <si>
+    <t>Cursed</t>
+  </si>
+  <si>
+    <t>Elements</t>
+  </si>
+  <si>
+    <t>Shoud classes restrict or augment equipment severely. Example, should the snake shift of druid not allow any equipment except for 3 bracers lol. Idk</t>
+  </si>
+  <si>
+    <t>Or things like a stance in berserker changes you to only be able to equip 1 2H weapon</t>
+  </si>
+  <si>
+    <t>Fist weapon classes</t>
+  </si>
+  <si>
+    <t>No weapon classes</t>
+  </si>
+  <si>
+    <t>No armor classes</t>
+  </si>
+  <si>
+    <t>No armor or weapon classes</t>
+  </si>
+  <si>
+    <t>This may allow for some more freedom in equipment if we don't have to worry about weird crossovers</t>
+  </si>
+  <si>
+    <t>It also doesn't make sense for a wolf to use a sword</t>
+  </si>
+  <si>
+    <t>Sniper</t>
+  </si>
+  <si>
+    <t>Gunslinger</t>
+  </si>
+  <si>
+    <t>Fencer</t>
+  </si>
+  <si>
+    <t>Brewmaster</t>
+  </si>
+  <si>
+    <t>Treant - Tank</t>
+  </si>
+  <si>
+    <t>Advanced Combat</t>
+  </si>
+  <si>
+    <t>Combos</t>
+  </si>
+  <si>
+    <t>Spells</t>
+  </si>
+  <si>
+    <t>Buffs</t>
+  </si>
+  <si>
+    <t>Temporary Perks</t>
+  </si>
+  <si>
+    <t>Gambler</t>
+  </si>
+  <si>
+    <t>Triggered events from combat rotation - Not sure what the hard limit should be 3 or 4 maybe 5 for some classes</t>
+  </si>
+  <si>
+    <t>Abilities like on ground effects casted from you spell book on to players, enemies, or ground. There should probably either be a lot of spells or a hihg combo cap for classes</t>
+  </si>
+  <si>
+    <t>Permanent buffs gathered from quests in the ranks of the particular class</t>
+  </si>
+  <si>
+    <t>Repeatable quest rewards that buff you temporarily. No cap</t>
+  </si>
+  <si>
+    <t>Food, elixirs, etc. All Temporary</t>
+  </si>
+  <si>
+    <t>Daily quests like bounty resets. You should be able to use a crafted item to boost dailies if you want</t>
+  </si>
+  <si>
+    <t>Combo Types</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Stacking</t>
+  </si>
+  <si>
+    <t>Ramping</t>
+  </si>
+  <si>
+    <t>Primers</t>
+  </si>
+  <si>
+    <t>Detonators</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Spell Types</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>AoE</t>
+  </si>
+  <si>
+    <t>Temporary Buffs / Debuffs</t>
+  </si>
+  <si>
+    <t>Hybrids</t>
+  </si>
+  <si>
+    <t>Telegraph</t>
+  </si>
+  <si>
+    <t>Junkie</t>
+  </si>
+  <si>
+    <t>Balancing</t>
+  </si>
+  <si>
+    <t>Skill Floor</t>
+  </si>
+  <si>
+    <t>Skill Ceiling</t>
+  </si>
+  <si>
+    <t>Passive Perks</t>
+  </si>
+  <si>
+    <t>Perk Choices</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>Costly</t>
+  </si>
+  <si>
+    <t>Wide</t>
+  </si>
+  <si>
+    <t>Narrow</t>
+  </si>
+  <si>
+    <t>Some gathering and crafting classes may make up some classes or at least sub classes</t>
+  </si>
+  <si>
+    <t>Class Pack Examples</t>
+  </si>
+  <si>
+    <t>Barbarian</t>
+  </si>
+  <si>
+    <t>Sub - Berserker</t>
+  </si>
+  <si>
+    <t>Sub - Brawler</t>
+  </si>
+  <si>
+    <t>Sub - Weapon Master</t>
+  </si>
+  <si>
+    <t>Sub - War Chief</t>
+  </si>
+  <si>
+    <t>Class Derivations</t>
+  </si>
+  <si>
+    <t>Start - Warrior</t>
+  </si>
+  <si>
+    <t>Sub</t>
+  </si>
+  <si>
+    <t>Deviation</t>
+  </si>
+  <si>
+    <t>Primal</t>
+  </si>
+  <si>
+    <t>Sub - Battlemind</t>
+  </si>
+  <si>
+    <t>Sub - Medic</t>
+  </si>
+  <si>
+    <t>Branch of Warrior with more emphasis on Primal aspects</t>
+  </si>
+  <si>
+    <t>Branch of Warrior with more emphasis on Martial and Military</t>
+  </si>
+  <si>
+    <t>Sub - Knight</t>
+  </si>
+  <si>
+    <t>Sub - Lancer</t>
+  </si>
+  <si>
+    <t>Sub - Commander</t>
+  </si>
+  <si>
+    <t>Attunement</t>
+  </si>
+  <si>
+    <t>Perk Select</t>
+  </si>
+  <si>
+    <t>Dual Wield | Mostly Combos - Few Spells</t>
+  </si>
+  <si>
+    <t>Fists, grappling | Balanced on Spells and Combos</t>
+  </si>
+  <si>
+    <t>2 Handed weapons | Mostly Combos</t>
+  </si>
+  <si>
+    <t>More buffs and control with aspects of all. Balanced. Maybe we have Hero classes or Legend classes</t>
+  </si>
+  <si>
+    <t>Sub - Tomahawk</t>
+  </si>
+  <si>
+    <t>Ranged warrior | Balanced</t>
+  </si>
+  <si>
+    <t>Sub - Gatling</t>
+  </si>
+  <si>
+    <t>Movement</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1391,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1171,6 +1481,29 @@
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
+    </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color rgb="FF92D050"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFF0000"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color rgb="FF92D050"/>
+        </stop>
+        <stop position="0.5">
+          <color rgb="FFFF0000"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF92D050"/>
+        </stop>
+      </gradientFill>
     </fill>
   </fills>
   <borders count="14">
@@ -1330,7 +1663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1386,6 +1719,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1407,6 +1752,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1420,6 +1771,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1970,62 +2324,62 @@
       <c r="A7" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="29"/>
+      <c r="C7" s="33"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35"/>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="C11" s="29"/>
+      <c r="C11" s="33"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="E14" s="27" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="E14" s="31" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="27"/>
+      <c r="E15" s="31"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="E16" s="27"/>
+      <c r="C16" s="33"/>
+      <c r="E16" s="31"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="E17" s="27"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
+      <c r="E17" s="31"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="27"/>
+      <c r="E18" s="31"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="27"/>
+      <c r="E19" s="31"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -2609,7 +2963,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,11 +2975,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="25" t="s">
         <v>264</v>
       </c>
@@ -2639,9 +2993,9 @@
       <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="25" t="s">
         <v>265</v>
       </c>
@@ -2655,10 +3009,12 @@
       <c r="L2" s="25"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="25"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="29" t="s">
+        <v>388</v>
+      </c>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
@@ -2669,9 +3025,9 @@
       <c r="L3" s="25"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
@@ -2683,9 +3039,9 @@
       <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
@@ -2902,10 +3258,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69264F54-9ABE-4235-8AC2-FF730385718C}">
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2932,106 +3288,106 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="29"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="33"/>
       <c r="G2" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="29"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="33"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="33"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="37"/>
       <c r="G3" s="13" t="s">
         <v>65</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="33"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="37"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="33"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="37"/>
       <c r="G4" s="11" t="s">
         <v>66</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="33"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="37"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="33"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="37"/>
       <c r="G5" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="33"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="37"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="33"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="33"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="37"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="33"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="33"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="37"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="37"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="31"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="33"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="35"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="37"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -3046,10 +3402,10 @@
       <c r="D9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="32"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="33"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="37"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -3067,10 +3423,10 @@
       <c r="G10" t="s">
         <v>91</v>
       </c>
-      <c r="K10" s="32"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="33"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="37"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -3085,14 +3441,14 @@
       <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="H11" s="38"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="33"/>
+      <c r="H11" s="44"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="37"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -3107,14 +3463,14 @@
       <c r="D12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="H12" s="38"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="33"/>
+      <c r="H12" s="44"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="37"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -3129,241 +3485,307 @@
       <c r="D13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="33"/>
+      <c r="H13" s="44"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="37"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="31"/>
+      <c r="H14" s="44"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="35"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="38"/>
+      <c r="H15" s="44"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="H16" s="38"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="44"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="H17" s="38"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="H17" s="44"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="29"/>
-      <c r="G18" s="38" t="s">
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="33"/>
+      <c r="G18" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="H18" s="38"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="33"/>
-      <c r="G19" s="38" t="s">
+      <c r="H18" s="44"/>
+      <c r="J18" s="45" t="s">
+        <v>403</v>
+      </c>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="37"/>
+      <c r="G19" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="H19" s="38"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="33"/>
-      <c r="G20" s="38" t="s">
+      <c r="H19" s="44"/>
+      <c r="J19" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="26" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="37"/>
+      <c r="G20" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="38"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="33"/>
-      <c r="G21" s="38" t="s">
+      <c r="H20" s="44"/>
+      <c r="J20" s="30" t="s">
+        <v>378</v>
+      </c>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="26" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="37"/>
+      <c r="G21" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="38"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="33"/>
-      <c r="G22" s="38" t="s">
+      <c r="H21" s="44"/>
+      <c r="J21" s="30" t="s">
+        <v>406</v>
+      </c>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="26" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="37"/>
+      <c r="G22" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="38"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="33"/>
-      <c r="G23" s="38" t="s">
+      <c r="H22" s="44"/>
+      <c r="J22" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="26" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="37"/>
+      <c r="G23" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="H23" s="38"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="33"/>
-      <c r="G24" s="38" t="s">
+      <c r="H23" s="44"/>
+      <c r="J23" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="26" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="37"/>
+      <c r="G24" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="H24" s="38"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="31"/>
-      <c r="G25" s="38" t="s">
+      <c r="H24" s="44"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="35"/>
+      <c r="G25" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="H25" s="38"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G26" s="38" t="s">
+      <c r="H25" s="44"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G26" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="38"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="44"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
       <c r="B27" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="G27" s="38" t="s">
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="G27" s="44" t="s">
         <v>266</v>
       </c>
-      <c r="H27" s="38"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="44"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="G28" s="38" t="s">
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="G28" s="44" t="s">
         <v>267</v>
       </c>
-      <c r="H28" s="38"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="44"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="G29" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="H29" s="44"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="G30" s="44" t="s">
+        <v>350</v>
+      </c>
+      <c r="H30" s="44"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="G31" s="44" t="s">
+        <v>351</v>
+      </c>
+      <c r="H31" s="44"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="G32" s="44" t="s">
+        <v>361</v>
+      </c>
+      <c r="H32" s="44"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -3372,13 +3794,15 @@
       <c r="B33" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="G33" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="H33" s="44"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -3387,13 +3811,15 @@
       <c r="B34" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="G34" s="44" t="s">
+        <v>363</v>
+      </c>
+      <c r="H34" s="44"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -3402,13 +3828,13 @@
       <c r="B35" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -3417,13 +3843,13 @@
       <c r="B36" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -3432,13 +3858,13 @@
       <c r="B37" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -3447,13 +3873,13 @@
       <c r="B38" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -3462,13 +3888,13 @@
       <c r="B39" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -3477,13 +3903,13 @@
       <c r="B40" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="34" t="s">
+      <c r="C40" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -3492,13 +3918,13 @@
       <c r="B41" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -3507,13 +3933,13 @@
       <c r="B42" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -3522,11 +3948,11 @@
       <c r="B43" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -3535,11 +3961,11 @@
       <c r="B44" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -3548,11 +3974,11 @@
       <c r="B45" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -3561,11 +3987,11 @@
       <c r="B46" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="34" t="s">
+      <c r="C46" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -3574,11 +4000,11 @@
       <c r="B47" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -3587,74 +4013,182 @@
       <c r="B48" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-    </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>339</v>
+      </c>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>340</v>
+      </c>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>341</v>
+      </c>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>342</v>
+      </c>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>343</v>
+      </c>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>344</v>
+      </c>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>345</v>
+      </c>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>346</v>
+      </c>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>347</v>
+      </c>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>348</v>
+      </c>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>349</v>
+      </c>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>402</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="69">
+  <mergeCells count="75">
     <mergeCell ref="G39:H39"/>
     <mergeCell ref="G40:H40"/>
     <mergeCell ref="G41:H41"/>
@@ -3696,6 +4230,8 @@
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="A2:E8"/>
     <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J18:O18"/>
+    <mergeCell ref="K23:N23"/>
     <mergeCell ref="C60:E60"/>
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="C39:E39"/>
@@ -3712,6 +4248,10 @@
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="C52:E52"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
     <mergeCell ref="C53:E53"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C33:E33"/>
@@ -3732,121 +4272,288 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3881CE4-01D8-42F0-A452-3448CAC129CD}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="77.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="D1" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="28"/>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="27"/>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="40"/>
-      <c r="D3" t="s">
+      <c r="N2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="47"/>
+      <c r="C3" s="27"/>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="40"/>
-      <c r="D4" t="s">
+      <c r="N3" t="s">
+        <v>421</v>
+      </c>
+      <c r="O3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="47"/>
+      <c r="C4" s="27"/>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="40"/>
-      <c r="D5" t="s">
+      <c r="N4" t="s">
+        <v>414</v>
+      </c>
+      <c r="O4" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="47"/>
+      <c r="C5" s="27"/>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="D6" t="s">
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="48"/>
+      <c r="C6" s="27"/>
+      <c r="E6" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="46" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="40"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="40"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="27"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="47"/>
+      <c r="C8" s="27"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="47"/>
+      <c r="C9" s="27"/>
+      <c r="E9" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="47"/>
+      <c r="C10" s="27"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="48"/>
+      <c r="C11" s="27"/>
+      <c r="D11" t="s">
+        <v>431</v>
+      </c>
+      <c r="E11" t="s">
+        <v>414</v>
+      </c>
+      <c r="F11" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="46" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="40"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="27"/>
+      <c r="D12" t="s">
+        <v>432</v>
+      </c>
+      <c r="E12" t="s">
+        <v>415</v>
+      </c>
+      <c r="F12" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="47"/>
+      <c r="C13" s="27"/>
+      <c r="D13" t="s">
+        <v>432</v>
+      </c>
+      <c r="E13" t="s">
+        <v>416</v>
+      </c>
+      <c r="F13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="47"/>
+      <c r="C14" s="27"/>
+      <c r="D14" t="s">
+        <v>432</v>
+      </c>
+      <c r="E14" t="s">
+        <v>417</v>
+      </c>
+      <c r="F14" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="47"/>
+      <c r="C15" s="27"/>
+      <c r="D15" t="s">
+        <v>432</v>
+      </c>
+      <c r="E15" t="s">
+        <v>418</v>
+      </c>
+      <c r="F15" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="48"/>
+      <c r="C16" s="27"/>
+      <c r="D16" t="s">
+        <v>432</v>
+      </c>
+      <c r="E16" t="s">
+        <v>437</v>
+      </c>
+      <c r="F16" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="46" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="40"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="40"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="40"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="41"/>
+      <c r="C17" s="27"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="47"/>
+      <c r="C18" s="27"/>
+      <c r="D18" t="s">
+        <v>431</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="47"/>
+      <c r="C19" s="27"/>
+      <c r="D19" t="s">
+        <v>432</v>
+      </c>
+      <c r="E19" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="47"/>
+      <c r="C20" s="27"/>
+      <c r="D20" t="s">
+        <v>432</v>
+      </c>
+      <c r="E20" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="48"/>
+      <c r="C21" s="27"/>
+      <c r="D21" t="s">
+        <v>432</v>
+      </c>
+      <c r="E21" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>432</v>
+      </c>
+      <c r="E22" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>412</v>
+      </c>
+      <c r="D23" t="s">
+        <v>432</v>
+      </c>
+      <c r="E23" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>432</v>
+      </c>
+      <c r="E24" t="s">
+        <v>439</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3862,10 +4569,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBD599A-923F-4747-99B7-36F41DFFA6EB}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3885,6 +4592,46 @@
         <v>333</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>371</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3892,10 +4639,142 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77303197-CDB9-4986-A878-7CD56B4A0DF4}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B4" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>381</v>
+      </c>
+      <c r="B6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>389</v>
+      </c>
+      <c r="B10" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>390</v>
+      </c>
+      <c r="B11" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>392</v>
+      </c>
+      <c r="B12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>391</v>
+      </c>
+      <c r="B13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>393</v>
+      </c>
+      <c r="B14" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>401</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603E61FB-347C-4063-9B10-037963F6D049}">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -3931,16 +4810,16 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="49" t="s">
         <v>294</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="51" t="s">
         <v>298</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="51" t="s">
         <v>297</v>
       </c>
       <c r="F4" t="str">
@@ -3949,46 +4828,46 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
       <c r="F5" t="str">
         <f>A8</f>
         <v>Instancing: Client - Dungeons / Zones</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
       <c r="F6" t="str">
         <f>A12</f>
         <v>Items on Ground</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
       <c r="F7" t="str">
         <f>A16</f>
         <v>Equipment Manager</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="49" t="s">
         <v>295</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="51" t="s">
         <v>299</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="51" t="s">
         <v>300</v>
       </c>
       <c r="F8" t="str">
@@ -3997,92 +4876,92 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
       <c r="F9" t="str">
         <f>A24</f>
         <v>Augmenting Equipment</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
       <c r="F10" t="str">
         <f>A28</f>
         <v>Perks Panel</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
       <c r="F11" t="str">
         <f>A32</f>
         <v>Perk Activate Panel - Equip</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="49" t="s">
         <v>282</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="51" t="s">
         <v>301</v>
       </c>
-      <c r="D12" s="44"/>
+      <c r="D12" s="51"/>
       <c r="F12" t="str">
         <f>A36</f>
         <v>Simple combat</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
       <c r="F13" t="str">
         <f>A44</f>
         <v>Advanced combat</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
       <c r="F14" t="str">
         <f>A48</f>
         <v>Gathering - Server</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
       <c r="F15" t="str">
         <f>A52</f>
         <v>Gathering - Client</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="49" t="s">
         <v>283</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="51" t="s">
         <v>302</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="51" t="s">
         <v>303</v>
       </c>
       <c r="F16" t="str">
@@ -4091,46 +4970,46 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
       <c r="F17" t="str">
         <f>A60</f>
         <v>Banking</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
       <c r="F18" t="str">
         <f>A64</f>
         <v>Quest Manager</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
       <c r="F19" t="str">
         <f>A68</f>
         <v>Spellbooks</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="49" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="51" t="s">
         <v>304</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="51" t="s">
         <v>305</v>
       </c>
       <c r="F20" t="str">
@@ -4139,494 +5018,494 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
       <c r="F21" t="str">
         <f>A76</f>
         <v>Camera Controls</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
       <c r="F22" t="str">
         <f>A80</f>
         <v>UI and Menus</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
+      <c r="A23" s="49"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="49" t="s">
         <v>285</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="51" t="s">
         <v>306</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="51" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
+      <c r="A27" s="49"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="51" t="s">
         <v>308</v>
       </c>
-      <c r="D28" s="44"/>
+      <c r="D28" s="51"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
+      <c r="A31" s="49"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="49" t="s">
         <v>287</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="51" t="s">
         <v>309</v>
       </c>
-      <c r="D32" s="44"/>
+      <c r="D32" s="51"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="51" t="s">
         <v>310</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="51" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="49" t="s">
         <v>312</v>
       </c>
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="51" t="s">
         <v>313</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D40" s="51" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
+      <c r="A42" s="49"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
+      <c r="A43" s="49"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="42" t="s">
+      <c r="A44" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C44" s="44" t="s">
+      <c r="C44" s="51" t="s">
         <v>315</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="51" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
+      <c r="A45" s="49"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="42"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
+      <c r="A47" s="49"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="42" t="s">
+      <c r="A48" s="49" t="s">
         <v>290</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C48" s="44" t="s">
+      <c r="C48" s="51" t="s">
         <v>317</v>
       </c>
-      <c r="D48" s="44"/>
+      <c r="D48" s="51"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="42"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
+      <c r="A49" s="49"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="42"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
+      <c r="A50" s="49"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="42"/>
-      <c r="B51" s="43"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44"/>
+      <c r="A51" s="49"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="42" t="s">
+      <c r="A52" s="49" t="s">
         <v>291</v>
       </c>
-      <c r="B52" s="43" t="s">
+      <c r="B52" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C52" s="51" t="s">
         <v>318</v>
       </c>
-      <c r="D52" s="44" t="s">
+      <c r="D52" s="51" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="42"/>
-      <c r="B53" s="43"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
+      <c r="A53" s="49"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="42"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="44"/>
-      <c r="D54" s="44"/>
+      <c r="A54" s="49"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="42"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="44"/>
-      <c r="D55" s="44"/>
+      <c r="A55" s="49"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="42" t="s">
+      <c r="A56" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C56" s="44" t="s">
+      <c r="C56" s="51" t="s">
         <v>320</v>
       </c>
-      <c r="D56" s="44" t="s">
+      <c r="D56" s="51" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="42"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
+      <c r="A57" s="49"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="51"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="42"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
+      <c r="A58" s="49"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="51"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="42"/>
-      <c r="B59" s="43"/>
-      <c r="C59" s="44"/>
-      <c r="D59" s="44"/>
+      <c r="A59" s="49"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="51"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="42" t="s">
+      <c r="A60" s="49" t="s">
         <v>292</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C60" s="44" t="s">
+      <c r="C60" s="51" t="s">
         <v>322</v>
       </c>
-      <c r="D60" s="44" t="s">
+      <c r="D60" s="51" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="42"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
+      <c r="A61" s="49"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="51"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="42"/>
-      <c r="B62" s="43"/>
-      <c r="C62" s="44"/>
-      <c r="D62" s="44"/>
+      <c r="A62" s="49"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="42"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
+      <c r="A63" s="49"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="51"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="42" t="s">
+      <c r="A64" s="49" t="s">
         <v>293</v>
       </c>
-      <c r="B64" s="43" t="s">
+      <c r="B64" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C64" s="44" t="s">
+      <c r="C64" s="51" t="s">
         <v>324</v>
       </c>
-      <c r="D64" s="44" t="s">
+      <c r="D64" s="51" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="42"/>
-      <c r="B65" s="43"/>
-      <c r="C65" s="44"/>
-      <c r="D65" s="44"/>
+      <c r="A65" s="49"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="51"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="42"/>
-      <c r="B66" s="43"/>
-      <c r="C66" s="44"/>
-      <c r="D66" s="44"/>
+      <c r="A66" s="49"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="42"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="44"/>
-      <c r="D67" s="44"/>
+      <c r="A67" s="49"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="51"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="42" t="s">
+      <c r="A68" s="49" t="s">
         <v>326</v>
       </c>
-      <c r="B68" s="43" t="s">
+      <c r="B68" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C68" s="44" t="s">
+      <c r="C68" s="51" t="s">
         <v>328</v>
       </c>
-      <c r="D68" s="44" t="s">
+      <c r="D68" s="51" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="42"/>
-      <c r="B69" s="43"/>
-      <c r="C69" s="44"/>
-      <c r="D69" s="44"/>
+      <c r="A69" s="49"/>
+      <c r="B69" s="50"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="42"/>
-      <c r="B70" s="43"/>
-      <c r="C70" s="44"/>
-      <c r="D70" s="44"/>
+      <c r="A70" s="49"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="51"/>
+      <c r="D70" s="51"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="42"/>
-      <c r="B71" s="43"/>
-      <c r="C71" s="44"/>
-      <c r="D71" s="44"/>
+      <c r="A71" s="49"/>
+      <c r="B71" s="50"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="51"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="42" t="s">
+      <c r="A72" s="49" t="s">
         <v>327</v>
       </c>
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C72" s="44" t="s">
+      <c r="C72" s="51" t="s">
         <v>330</v>
       </c>
-      <c r="D72" s="44"/>
+      <c r="D72" s="51"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="42"/>
-      <c r="B73" s="43"/>
-      <c r="C73" s="44"/>
-      <c r="D73" s="44"/>
+      <c r="A73" s="49"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="51"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="42"/>
-      <c r="B74" s="43"/>
-      <c r="C74" s="44"/>
-      <c r="D74" s="44"/>
+      <c r="A74" s="49"/>
+      <c r="B74" s="50"/>
+      <c r="C74" s="51"/>
+      <c r="D74" s="51"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="42"/>
-      <c r="B75" s="43"/>
-      <c r="C75" s="44"/>
-      <c r="D75" s="44"/>
+      <c r="A75" s="49"/>
+      <c r="B75" s="50"/>
+      <c r="C75" s="51"/>
+      <c r="D75" s="51"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="42" t="s">
+      <c r="A76" s="49" t="s">
         <v>336</v>
       </c>
-      <c r="B76" s="43" t="s">
+      <c r="B76" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C76" s="44"/>
-      <c r="D76" s="44"/>
+      <c r="C76" s="51"/>
+      <c r="D76" s="51"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="42"/>
-      <c r="B77" s="43"/>
-      <c r="C77" s="44"/>
-      <c r="D77" s="44"/>
+      <c r="A77" s="49"/>
+      <c r="B77" s="50"/>
+      <c r="C77" s="51"/>
+      <c r="D77" s="51"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="42"/>
-      <c r="B78" s="43"/>
-      <c r="C78" s="44"/>
-      <c r="D78" s="44"/>
+      <c r="A78" s="49"/>
+      <c r="B78" s="50"/>
+      <c r="C78" s="51"/>
+      <c r="D78" s="51"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="42"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="44"/>
-      <c r="D79" s="44"/>
+      <c r="A79" s="49"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="51"/>
+      <c r="D79" s="51"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="42" t="s">
+      <c r="A80" s="49" t="s">
         <v>337</v>
       </c>
-      <c r="B80" s="43" t="s">
+      <c r="B80" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="C80" s="44"/>
-      <c r="D80" s="44"/>
+      <c r="C80" s="51"/>
+      <c r="D80" s="51"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="42"/>
-      <c r="B81" s="43"/>
-      <c r="C81" s="44"/>
-      <c r="D81" s="44"/>
+      <c r="A81" s="49"/>
+      <c r="B81" s="50"/>
+      <c r="C81" s="51"/>
+      <c r="D81" s="51"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="42"/>
-      <c r="B82" s="43"/>
-      <c r="C82" s="44"/>
-      <c r="D82" s="44"/>
+      <c r="A82" s="49"/>
+      <c r="B82" s="50"/>
+      <c r="C82" s="51"/>
+      <c r="D82" s="51"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="42"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="44"/>
-      <c r="D83" s="44"/>
+      <c r="A83" s="49"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="51"/>
+      <c r="D83" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="80">

</xml_diff>

<commit_message>
Latest Update - Stats and Equipment
</commit_message>
<xml_diff>
--- a/Game Theory.xlsx
+++ b/Game Theory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public-Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDD609C-8F41-4B8D-BC06-95C0826F5EB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FC3298-3EC5-492B-BA29-DC24A46051D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="689" firstSheet="2" activeTab="11" xr2:uid="{A1BE79B9-B4EE-42B4-9FA0-1B70B1F5C2B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="689" firstSheet="2" activeTab="8" xr2:uid="{A1BE79B9-B4EE-42B4-9FA0-1B70B1F5C2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats - General" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="906">
   <si>
     <t>Strength</t>
   </si>
@@ -2693,6 +2693,75 @@
   </si>
   <si>
     <t>Current Hits / Max Hits &lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt; DELAYED / Updated on Hit / Damage / Heal</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Slot Number</t>
+  </si>
+  <si>
+    <t>Neck</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Shoulders</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Wrist1</t>
+  </si>
+  <si>
+    <t>Writst2</t>
+  </si>
+  <si>
+    <t>Hands1</t>
+  </si>
+  <si>
+    <t>Hands2</t>
+  </si>
+  <si>
+    <t>Belt</t>
+  </si>
+  <si>
+    <t>Legs1</t>
+  </si>
+  <si>
+    <t>Legs2</t>
+  </si>
+  <si>
+    <t>Boots1</t>
+  </si>
+  <si>
+    <t>Boots2</t>
+  </si>
+  <si>
+    <t>Head2</t>
+  </si>
+  <si>
+    <t>Head1</t>
+  </si>
+  <si>
+    <t>1HW1</t>
+  </si>
+  <si>
+    <t>1HW2</t>
+  </si>
+  <si>
+    <t>2HW1</t>
+  </si>
+  <si>
+    <t>2HW2</t>
+  </si>
+  <si>
+    <t>Accessory1</t>
+  </si>
+  <si>
+    <t>Accessory2</t>
   </si>
 </sst>
 </file>
@@ -3208,20 +3277,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3232,10 +3289,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3389,16 +3458,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>421735</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>108860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>433969</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>188100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>2730</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3427,8 +3496,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="-772416" y="3477516"/>
-          <a:ext cx="6255525" cy="4691644"/>
+          <a:off x="2559459" y="3619461"/>
+          <a:ext cx="6751870" cy="5064667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5470,18 +5539,74 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="B104:B107"/>
-    <mergeCell ref="C104:C107"/>
-    <mergeCell ref="D104:D107"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
     <mergeCell ref="A88:A91"/>
     <mergeCell ref="B88:B91"/>
     <mergeCell ref="C88:C91"/>
@@ -5506,74 +5631,18 @@
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="D16:D19"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="C104:C107"/>
+    <mergeCell ref="D104:D107"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="D96:D99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5583,7 +5652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB6A08E-A9A6-467B-8DE6-4224317EBD93}">
   <dimension ref="A2:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -6491,9 +6560,9 @@
       <c r="A2" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="45"/>
       <c r="G2" s="8" t="s">
         <v>30</v>
@@ -6504,15 +6573,15 @@
       <c r="K2" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
       <c r="N2" s="45"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="48"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
       <c r="E3" s="49"/>
       <c r="G3" s="13" t="s">
         <v>62</v>
@@ -6521,15 +6590,15 @@
         <v>64</v>
       </c>
       <c r="K3" s="48"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
       <c r="N3" s="49"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="48"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="49"/>
       <c r="G4" s="11" t="s">
         <v>63</v>
@@ -6538,55 +6607,55 @@
         <v>65</v>
       </c>
       <c r="K4" s="48"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
       <c r="N4" s="49"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="48"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="49"/>
       <c r="G5" s="14" t="s">
         <v>81</v>
       </c>
       <c r="K5" s="48"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
       <c r="N5" s="49"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="48"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="49"/>
       <c r="K6" s="48"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="61"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
       <c r="N6" s="49"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="48"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
       <c r="E7" s="49"/>
       <c r="K7" s="48"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
       <c r="N7" s="49"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="46"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
       <c r="E8" s="47"/>
       <c r="K8" s="48"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
       <c r="N8" s="49"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -6603,8 +6672,8 @@
         <v>4</v>
       </c>
       <c r="K9" s="48"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="57"/>
       <c r="N9" s="49"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -6620,13 +6689,13 @@
       <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="64" t="s">
+      <c r="G10" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="64"/>
+      <c r="H10" s="61"/>
       <c r="K10" s="48"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="61"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
       <c r="N10" s="49"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -6642,13 +6711,13 @@
       <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="58"/>
+      <c r="H11" s="55"/>
       <c r="K11" s="48"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
       <c r="N11" s="49"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -6664,13 +6733,13 @@
       <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="H12" s="58"/>
+      <c r="H12" s="55"/>
       <c r="K12" s="48"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="61"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
       <c r="N12" s="49"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -6686,13 +6755,13 @@
       <c r="D13" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="H13" s="58"/>
+      <c r="H13" s="55"/>
       <c r="K13" s="48"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="61"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
       <c r="N13" s="49"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -6700,13 +6769,13 @@
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H14" s="58"/>
+      <c r="H14" s="55"/>
       <c r="K14" s="46"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
       <c r="N14" s="47"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -6714,25 +6783,25 @@
       <c r="B15" s="36"/>
       <c r="C15" s="36"/>
       <c r="D15" s="36"/>
-      <c r="G15" s="58" t="s">
+      <c r="G15" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="H15" s="58"/>
+      <c r="H15" s="55"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G16" s="58" t="s">
+      <c r="G16" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="H16" s="58"/>
+      <c r="H16" s="55"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="H17" s="58"/>
+      <c r="H17" s="55"/>
       <c r="J17" t="s">
         <v>493</v>
       </c>
@@ -6741,97 +6810,97 @@
       <c r="A18" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="45"/>
-      <c r="G18" s="58" t="s">
+      <c r="G18" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="H18" s="58"/>
+      <c r="H18" s="55"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="48"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="49"/>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="H19" s="58"/>
+      <c r="H19" s="55"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="48"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="49"/>
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="H20" s="58"/>
+      <c r="H20" s="55"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="48"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="49"/>
-      <c r="G21" s="58" t="s">
+      <c r="G21" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="H21" s="58"/>
+      <c r="H21" s="55"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="48"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="49"/>
-      <c r="G22" s="58" t="s">
+      <c r="G22" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="H22" s="58"/>
+      <c r="H22" s="55"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="48"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="49"/>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="H23" s="58"/>
+      <c r="H23" s="55"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="48"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="49"/>
-      <c r="G24" s="58" t="s">
+      <c r="G24" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="H24" s="58"/>
+      <c r="H24" s="55"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
       <c r="E25" s="47"/>
-      <c r="G25" s="58" t="s">
+      <c r="G25" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="H25" s="58"/>
+      <c r="H25" s="55"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G26" s="58" t="s">
+      <c r="G26" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="H26" s="58"/>
+      <c r="H26" s="55"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -6840,15 +6909,15 @@
       <c r="B27" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="G27" s="58" t="s">
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="G27" s="55" t="s">
         <v>262</v>
       </c>
-      <c r="H27" s="58"/>
+      <c r="H27" s="55"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -6857,15 +6926,15 @@
       <c r="B28" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="C28" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="G28" s="58" t="s">
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="G28" s="55" t="s">
         <v>263</v>
       </c>
-      <c r="H28" s="58"/>
+      <c r="H28" s="55"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -6874,15 +6943,15 @@
       <c r="B29" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="G29" s="58" t="s">
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="G29" s="55" t="s">
         <v>334</v>
       </c>
-      <c r="H29" s="58"/>
+      <c r="H29" s="55"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -6891,15 +6960,15 @@
       <c r="B30" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="G30" s="58" t="s">
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="G30" s="55" t="s">
         <v>346</v>
       </c>
-      <c r="H30" s="58"/>
+      <c r="H30" s="55"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -6908,15 +6977,15 @@
       <c r="B31" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="G31" s="58" t="s">
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="G31" s="55" t="s">
         <v>347</v>
       </c>
-      <c r="H31" s="58"/>
+      <c r="H31" s="55"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -6925,23 +6994,23 @@
       <c r="B32" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="57" t="s">
+      <c r="C32" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="G32" s="58" t="s">
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="G32" s="55" t="s">
         <v>357</v>
       </c>
-      <c r="H32" s="58"/>
-      <c r="J32" s="63" t="s">
+      <c r="H32" s="55"/>
+      <c r="J32" s="60" t="s">
         <v>399</v>
       </c>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -6950,22 +7019,22 @@
       <c r="B33" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="57" t="s">
+      <c r="C33" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
-      <c r="G33" s="58" t="s">
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="G33" s="55" t="s">
         <v>358</v>
       </c>
-      <c r="H33" s="58"/>
+      <c r="H33" s="55"/>
       <c r="J33" s="30" t="s">
         <v>400</v>
       </c>
-      <c r="K33" s="55"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="55"/>
-      <c r="N33" s="55"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="62"/>
+      <c r="N33" s="62"/>
       <c r="O33" s="26" t="s">
         <v>401</v>
       </c>
@@ -6977,22 +7046,22 @@
       <c r="B34" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="57" t="s">
+      <c r="C34" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="G34" s="58" t="s">
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="G34" s="55" t="s">
         <v>359</v>
       </c>
-      <c r="H34" s="58"/>
+      <c r="H34" s="55"/>
       <c r="J34" s="30" t="s">
         <v>374</v>
       </c>
-      <c r="K34" s="56"/>
-      <c r="L34" s="56"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="56"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="64"/>
+      <c r="N34" s="64"/>
       <c r="O34" s="26" t="s">
         <v>375</v>
       </c>
@@ -7004,22 +7073,22 @@
       <c r="B35" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="57" t="s">
+      <c r="C35" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
-      <c r="G35" s="58" t="s">
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="G35" s="55" t="s">
         <v>490</v>
       </c>
-      <c r="H35" s="58"/>
+      <c r="H35" s="55"/>
       <c r="J35" s="30" t="s">
         <v>402</v>
       </c>
-      <c r="K35" s="55"/>
-      <c r="L35" s="55"/>
-      <c r="M35" s="55"/>
-      <c r="N35" s="55"/>
+      <c r="K35" s="62"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="62"/>
+      <c r="N35" s="62"/>
       <c r="O35" s="26" t="s">
         <v>403</v>
       </c>
@@ -7031,22 +7100,22 @@
       <c r="B36" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="57" t="s">
+      <c r="C36" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="G36" s="58" t="s">
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="G36" s="55" t="s">
         <v>491</v>
       </c>
-      <c r="H36" s="58"/>
+      <c r="H36" s="55"/>
       <c r="J36" s="30" t="s">
         <v>404</v>
       </c>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
       <c r="O36" s="26" t="s">
         <v>405</v>
       </c>
@@ -7058,22 +7127,22 @@
       <c r="B37" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="57" t="s">
+      <c r="C37" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="G37" s="58" t="s">
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="G37" s="55" t="s">
         <v>492</v>
       </c>
-      <c r="H37" s="58"/>
+      <c r="H37" s="55"/>
       <c r="J37" s="30" t="s">
         <v>406</v>
       </c>
-      <c r="K37" s="55"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="55"/>
-      <c r="N37" s="55"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="62"/>
+      <c r="M37" s="62"/>
+      <c r="N37" s="62"/>
       <c r="O37" s="26" t="s">
         <v>407</v>
       </c>
@@ -7085,13 +7154,13 @@
       <c r="B38" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="57" t="s">
+      <c r="C38" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="55"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -7100,13 +7169,13 @@
       <c r="B39" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="57" t="s">
+      <c r="C39" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -7115,13 +7184,13 @@
       <c r="B40" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="57" t="s">
+      <c r="C40" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D40" s="57"/>
-      <c r="E40" s="57"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -7130,13 +7199,13 @@
       <c r="B41" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="57" t="s">
+      <c r="C41" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -7145,13 +7214,13 @@
       <c r="B42" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="57" t="s">
+      <c r="C42" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -7160,11 +7229,11 @@
       <c r="B43" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="57" t="s">
+      <c r="C43" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -7173,11 +7242,11 @@
       <c r="B44" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C44" s="57" t="s">
+      <c r="C44" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -7186,11 +7255,11 @@
       <c r="B45" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="57" t="s">
+      <c r="C45" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -7199,11 +7268,11 @@
       <c r="B46" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="57" t="s">
+      <c r="C46" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -7212,11 +7281,11 @@
       <c r="B47" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="57" t="s">
+      <c r="C47" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -7225,16 +7294,16 @@
       <c r="B48" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="57" t="s">
+      <c r="C48" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C49" s="57"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="57"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
       <c r="F49" t="s">
         <v>350</v>
       </c>
@@ -7243,9 +7312,9 @@
       <c r="B50" t="s">
         <v>335</v>
       </c>
-      <c r="C50" s="57"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
       <c r="F50" t="s">
         <v>351</v>
       </c>
@@ -7254,9 +7323,9 @@
       <c r="B51" t="s">
         <v>336</v>
       </c>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
       <c r="F51" t="s">
         <v>353</v>
       </c>
@@ -7265,9 +7334,9 @@
       <c r="B52" t="s">
         <v>337</v>
       </c>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="59"/>
       <c r="F52" t="s">
         <v>354</v>
       </c>
@@ -7276,9 +7345,9 @@
       <c r="B53" t="s">
         <v>338</v>
       </c>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="57"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
       <c r="F53" t="s">
         <v>355</v>
       </c>
@@ -7287,41 +7356,41 @@
       <c r="B54" t="s">
         <v>339</v>
       </c>
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
+      <c r="C54" s="59"/>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>340</v>
       </c>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
+      <c r="C55" s="59"/>
+      <c r="D55" s="59"/>
+      <c r="E55" s="59"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>341</v>
       </c>
-      <c r="C56" s="57"/>
-      <c r="D56" s="57"/>
-      <c r="E56" s="57"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="59"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>342</v>
       </c>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="57"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>343</v>
       </c>
-      <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="57"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
       <c r="F58" t="s">
         <v>494</v>
       </c>
@@ -7331,28 +7400,28 @@
       <c r="J58" t="s">
         <v>500</v>
       </c>
-      <c r="K58" s="59" t="s">
+      <c r="K58" s="63" t="s">
         <v>501</v>
       </c>
-      <c r="L58" s="59"/>
-      <c r="M58" s="59"/>
-      <c r="N58" s="59"/>
+      <c r="L58" s="63"/>
+      <c r="M58" s="63"/>
+      <c r="N58" s="63"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>344</v>
       </c>
-      <c r="C59" s="57"/>
-      <c r="D59" s="57"/>
-      <c r="E59" s="57"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="59"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>345</v>
       </c>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
       <c r="F60" t="s">
         <v>495</v>
       </c>
@@ -7736,13 +7805,60 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="K36:N36"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="K2:N14"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A2:E8"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J32:O32"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="A18:E25"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
@@ -7759,60 +7875,13 @@
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="G28:H28"/>
-    <mergeCell ref="K2:N14"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="A2:E8"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J32:O32"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="K36:N36"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="K58:N58"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7840,10 +7909,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="55"/>
       <c r="C1" s="35"/>
       <c r="D1" s="28"/>
       <c r="E1" t="s">
@@ -9723,21 +9792,25 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A224:C224"/>
+    <mergeCell ref="A225:C225"/>
+    <mergeCell ref="A231:C231"/>
+    <mergeCell ref="A237:C237"/>
+    <mergeCell ref="A205:C205"/>
+    <mergeCell ref="A206:C206"/>
+    <mergeCell ref="A217:C217"/>
+    <mergeCell ref="A211:C211"/>
+    <mergeCell ref="A141:C141"/>
+    <mergeCell ref="A145:C145"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="A201:C201"/>
+    <mergeCell ref="A182:C182"/>
+    <mergeCell ref="A169:C169"/>
+    <mergeCell ref="A175:C175"/>
+    <mergeCell ref="A189:C189"/>
+    <mergeCell ref="A194:C194"/>
+    <mergeCell ref="A151:C151"/>
+    <mergeCell ref="A156:C156"/>
     <mergeCell ref="A83:C83"/>
     <mergeCell ref="A200:C200"/>
     <mergeCell ref="A181:C181"/>
@@ -9754,25 +9827,21 @@
     <mergeCell ref="A126:C126"/>
     <mergeCell ref="A135:C135"/>
     <mergeCell ref="A138:C138"/>
-    <mergeCell ref="A141:C141"/>
-    <mergeCell ref="A145:C145"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="A201:C201"/>
-    <mergeCell ref="A182:C182"/>
-    <mergeCell ref="A169:C169"/>
-    <mergeCell ref="A175:C175"/>
-    <mergeCell ref="A189:C189"/>
-    <mergeCell ref="A194:C194"/>
-    <mergeCell ref="A151:C151"/>
-    <mergeCell ref="A156:C156"/>
-    <mergeCell ref="A224:C224"/>
-    <mergeCell ref="A225:C225"/>
-    <mergeCell ref="A231:C231"/>
-    <mergeCell ref="A237:C237"/>
-    <mergeCell ref="A205:C205"/>
-    <mergeCell ref="A206:C206"/>
-    <mergeCell ref="A217:C217"/>
-    <mergeCell ref="A211:C211"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9781,13 +9850,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBD599A-923F-4747-99B7-36F41DFFA6EB}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -9842,6 +9915,182 @@
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>367</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>884</v>
+      </c>
+      <c r="B17" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>